<commit_message>
student model update. Start of new semester.
</commit_message>
<xml_diff>
--- a/data_FontysCampus/Buildings_FontysCampus.xlsx
+++ b/data_FontysCampus/Buildings_FontysCampus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Fontys_Campus\data_FontysCampus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys-my.sharepoint.com/personal/487503_student_fontys_nl/Documents/School/Fontys/Semester 6/ZEnmO/Model/Oefenmodel ZEnmO/Model/Fontys_Campus-main/Fontys_Campus-main/data_FontysCampus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492ED60-4BFD-4774-A640-CED29D1CF5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{C492ED60-4BFD-4774-A640-CED29D1CF5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F02C2AF-3ACE-4C9C-801F-E7BBB9E14582}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{99A50208-934F-4EDD-BF51-6D238E9C57FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99A50208-934F-4EDD-BF51-6D238E9C57FC}"/>
   </bookViews>
   <sheets>
     <sheet name="buildings" sheetId="4" r:id="rId1"/>
@@ -722,7 +722,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>polygon</t>
   </si>
@@ -884,13 +884,22 @@
   </si>
   <si>
     <t>r13</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>r9</t>
+  </si>
+  <si>
+    <t>parkeergarage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -911,6 +920,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -920,7 +935,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -958,11 +973,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -972,6 +1007,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1308,42 +1352,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD9D70-6DEB-4390-947E-55D38CEBDCD5}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="129.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="129.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1423,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>772010001072407</v>
       </c>
@@ -1489,7 +1533,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>772010001072406</v>
       </c>
@@ -1555,7 +1599,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>772010001072408</v>
       </c>
@@ -1619,7 +1663,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>772010001072409</v>
       </c>
@@ -1683,7 +1727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>772010001074106</v>
       </c>
@@ -1747,7 +1791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>772010001074107</v>
       </c>
@@ -1811,7 +1855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>772010001074108</v>
       </c>
@@ -1875,6 +1919,50 @@
         <v>40</v>
       </c>
     </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>772100001027963</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" s="6">
+        <v>51.451071839313101</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>5.4821012623284604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V11" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>